<commit_message>
Implementação do Extent Report
</commit_message>
<xml_diff>
--- a/src/main/resources/TestDataMobile.xlsx
+++ b/src/main/resources/TestDataMobile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willian.costa\eclipse-workspace\servlets\hub_tdd_mobile\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90F3C04-6798-4A21-A63E-F43AC0633B84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5EFFBA-96AB-4A7B-BBA4-3C5DAE7CE665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{9A238A30-1AA3-4A42-BD5B-6DAF71D155B8}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9A238A30-1AA3-4A42-BD5B-6DAF71D155B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>HP Z4000 WIRELESS MOUSE</t>
   </si>
   <si>
-    <t>joao123998877</t>
-  </si>
-  <si>
     <t>categoria</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>HP CHROMEBOOK 14 G1(ENERGY STAR)</t>
+  </si>
+  <si>
+    <t>joao123998</t>
   </si>
 </sst>
 </file>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047BA368-A67D-4FA4-AECD-0DBBBDE775BB}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0129FF7C-98B6-4340-B073-29657B0AE79B}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,10 +766,10 @@
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -780,10 +780,10 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -795,10 +795,10 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -809,10 +809,10 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,10 +823,10 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -835,20 +835,20 @@
       </c>
       <c r="B8" s="6"/>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>